<commit_message>
documentation now on tier1
</commit_message>
<xml_diff>
--- a/Documentation/ListOfPlugins.xlsx
+++ b/Documentation/ListOfPlugins.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2aec92b61cf85839/Projects/SMAP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonasries/git/SMAP/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{01790E50-1C15-4D4D-A5A9-D16230DFCCE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{4759AF1C-923E-4843-B0AF-F6F6849CF808}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAC581F-608F-2646-9DAD-89227B396F23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="17840" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="585">
   <si>
     <t>REFERENCE</t>
   </si>
@@ -2207,7 +2207,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0."/>
+    <numFmt numFmtId="164" formatCode="0."/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -2427,14 +2427,8 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2442,11 +2436,17 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2764,8 +2764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMF312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A294" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B301" sqref="B301:D301"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5862,10 +5862,10 @@
       <c r="AMF5" s="25"/>
     </row>
     <row r="6" spans="1:1020" s="22" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="19" t="s">
         <v>148</v>
       </c>
@@ -6888,10 +6888,10 @@
       <c r="AMF6" s="21"/>
     </row>
     <row r="7" spans="1:1020" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="33"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="5" t="s">
         <v>149</v>
       </c>
@@ -6969,10 +6969,10 @@
       </c>
     </row>
     <row r="15" spans="1:1020" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="33"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="4" t="s">
         <v>150</v>
       </c>
@@ -7062,10 +7062,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="33"/>
+      <c r="B23" s="36"/>
       <c r="C23" s="4" t="s">
         <v>151</v>
       </c>
@@ -7160,10 +7160,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="33"/>
+      <c r="B32" s="36"/>
       <c r="C32" s="4" t="s">
         <v>152</v>
       </c>
@@ -7270,10 +7270,10 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="33" t="s">
+      <c r="A41" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="33"/>
+      <c r="B41" s="36"/>
       <c r="C41" s="4" t="s">
         <v>165</v>
       </c>
@@ -7351,10 +7351,10 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="33" t="s">
+      <c r="A49" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="B49" s="33"/>
+      <c r="B49" s="36"/>
       <c r="C49" s="4" t="s">
         <v>31</v>
       </c>
@@ -7432,10 +7432,10 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="33" t="s">
+      <c r="A57" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B57" s="33"/>
+      <c r="B57" s="36"/>
       <c r="C57" s="1"/>
     </row>
     <row r="58" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -7511,10 +7511,10 @@
       </c>
     </row>
     <row r="65" spans="1:1020" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="34" t="s">
+      <c r="A65" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="B65" s="34"/>
+      <c r="B65" s="39"/>
       <c r="C65" s="4" t="s">
         <v>198</v>
       </c>
@@ -7562,10 +7562,10 @@
       </c>
     </row>
     <row r="70" spans="1:1020" s="22" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A70" s="35" t="s">
+      <c r="A70" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="B70" s="35"/>
+      <c r="B70" s="37"/>
       <c r="C70" s="19" t="s">
         <v>202</v>
       </c>
@@ -8588,10 +8588,10 @@
       <c r="AMF70" s="21"/>
     </row>
     <row r="71" spans="1:1020" x14ac:dyDescent="0.2">
-      <c r="A71" s="33" t="s">
+      <c r="A71" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="B71" s="33"/>
+      <c r="B71" s="36"/>
       <c r="C71" s="5" t="s">
         <v>579</v>
       </c>
@@ -8691,10 +8691,10 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="33" t="s">
+      <c r="A81" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B81" s="33"/>
+      <c r="B81" s="36"/>
       <c r="C81" s="5" t="s">
         <v>578</v>
       </c>
@@ -8771,10 +8771,10 @@
       <c r="D88" s="16"/>
     </row>
     <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" s="33" t="s">
+      <c r="A89" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B89" s="33"/>
+      <c r="B89" s="36"/>
       <c r="C89" s="4" t="s">
         <v>221</v>
       </c>
@@ -8888,10 +8888,10 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" s="33" t="s">
+      <c r="A100" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B100" s="33"/>
+      <c r="B100" s="36"/>
       <c r="C100" s="5" t="s">
         <v>577</v>
       </c>
@@ -8958,10 +8958,10 @@
       </c>
     </row>
     <row r="107" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" s="33" t="s">
+      <c r="A107" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="B107" s="33"/>
+      <c r="B107" s="36"/>
       <c r="C107" s="4" t="s">
         <v>222</v>
       </c>
@@ -8978,10 +8978,10 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A109" s="33" t="s">
+      <c r="A109" s="36" t="s">
         <v>576</v>
       </c>
-      <c r="B109" s="33"/>
+      <c r="B109" s="36"/>
       <c r="C109" s="5" t="s">
         <v>57</v>
       </c>
@@ -9065,10 +9065,10 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A117" s="33" t="s">
+      <c r="A117" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="B117" s="33"/>
+      <c r="B117" s="36"/>
       <c r="C117" s="1"/>
     </row>
     <row r="118" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -9098,6 +9098,9 @@
       <c r="C120" s="2" t="s">
         <v>247</v>
       </c>
+      <c r="D120" s="2" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="121" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
@@ -9144,10 +9147,10 @@
       </c>
     </row>
     <row r="125" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A125" s="33" t="s">
+      <c r="A125" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="B125" s="33"/>
+      <c r="B125" s="36"/>
       <c r="C125" s="4" t="s">
         <v>453</v>
       </c>
@@ -9335,10 +9338,10 @@
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A143" s="33" t="s">
+      <c r="A143" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="B143" s="33"/>
+      <c r="B143" s="36"/>
       <c r="C143" s="1"/>
     </row>
     <row r="144" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -9488,10 +9491,10 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A157" s="33" t="s">
+      <c r="A157" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="B157" s="33"/>
+      <c r="B157" s="36"/>
       <c r="C157" s="1"/>
     </row>
     <row r="158" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -9539,10 +9542,10 @@
       </c>
     </row>
     <row r="162" spans="1:1020" s="22" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A162" s="35" t="s">
+      <c r="A162" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B162" s="35"/>
+      <c r="B162" s="37"/>
       <c r="C162" s="27" t="s">
         <v>564</v>
       </c>
@@ -10565,10 +10568,10 @@
       <c r="AMF162" s="21"/>
     </row>
     <row r="163" spans="1:1020" x14ac:dyDescent="0.2">
-      <c r="A163" s="33" t="s">
+      <c r="A163" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="B163" s="33"/>
+      <c r="B163" s="36"/>
       <c r="C163" s="5" t="s">
         <v>565</v>
       </c>
@@ -10674,10 +10677,10 @@
       </c>
     </row>
     <row r="173" spans="1:1020" ht="17" x14ac:dyDescent="0.2">
-      <c r="A173" s="33" t="s">
+      <c r="A173" s="36" t="s">
         <v>422</v>
       </c>
-      <c r="B173" s="33"/>
+      <c r="B173" s="36"/>
       <c r="C173" s="3" t="s">
         <v>285</v>
       </c>
@@ -10753,10 +10756,10 @@
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A180" s="33" t="s">
+      <c r="A180" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="B180" s="33"/>
+      <c r="B180" s="36"/>
       <c r="C180" s="5" t="s">
         <v>574</v>
       </c>
@@ -10823,10 +10826,10 @@
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A187" s="33" t="s">
+      <c r="A187" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="B187" s="33"/>
+      <c r="B187" s="36"/>
       <c r="C187" s="11" t="s">
         <v>566</v>
       </c>
@@ -11038,10 +11041,10 @@
       </c>
     </row>
     <row r="205" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A205" s="34" t="s">
+      <c r="A205" s="39" t="s">
         <v>316</v>
       </c>
-      <c r="B205" s="34"/>
+      <c r="B205" s="39"/>
       <c r="C205" s="4" t="s">
         <v>467</v>
       </c>
@@ -11075,10 +11078,10 @@
       </c>
     </row>
     <row r="209" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A209" s="34" t="s">
+      <c r="A209" s="39" t="s">
         <v>510</v>
       </c>
-      <c r="B209" s="34"/>
+      <c r="B209" s="39"/>
       <c r="C209" s="4" t="s">
         <v>511</v>
       </c>
@@ -11132,10 +11135,10 @@
       </c>
     </row>
     <row r="214" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A214" s="34" t="s">
+      <c r="A214" s="39" t="s">
         <v>520</v>
       </c>
-      <c r="B214" s="34"/>
+      <c r="B214" s="39"/>
       <c r="C214" s="4" t="s">
         <v>521</v>
       </c>
@@ -11163,10 +11166,10 @@
       </c>
     </row>
     <row r="217" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A217" s="33" t="s">
+      <c r="A217" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="B217" s="33"/>
+      <c r="B217" s="36"/>
       <c r="C217" s="4" t="s">
         <v>308</v>
       </c>
@@ -11280,10 +11283,10 @@
       </c>
     </row>
     <row r="228" spans="1:1020" s="22" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A228" s="35" t="s">
+      <c r="A228" s="37" t="s">
         <v>540</v>
       </c>
-      <c r="B228" s="35"/>
+      <c r="B228" s="37"/>
       <c r="C228" s="27" t="s">
         <v>541</v>
       </c>
@@ -12323,10 +12326,10 @@
       </c>
     </row>
     <row r="231" spans="1:1020" ht="17" x14ac:dyDescent="0.2">
-      <c r="A231" s="33" t="s">
+      <c r="A231" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="B231" s="33"/>
+      <c r="B231" s="36"/>
       <c r="C231" s="4" t="s">
         <v>329</v>
       </c>
@@ -12515,10 +12518,10 @@
       </c>
     </row>
     <row r="248" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A248" s="33" t="s">
+      <c r="A248" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="B248" s="33"/>
+      <c r="B248" s="36"/>
       <c r="C248" s="4" t="s">
         <v>343</v>
       </c>
@@ -12751,10 +12754,10 @@
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A269" s="33" t="s">
+      <c r="A269" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="B269" s="33"/>
+      <c r="B269" s="36"/>
       <c r="C269" s="5" t="s">
         <v>569</v>
       </c>
@@ -12888,10 +12891,10 @@
       </c>
     </row>
     <row r="281" spans="1:1020" s="22" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A281" s="35" t="s">
+      <c r="A281" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="B281" s="35"/>
+      <c r="B281" s="37"/>
       <c r="C281" s="29" t="s">
         <v>570</v>
       </c>
@@ -13974,217 +13977,257 @@
       </c>
     </row>
     <row r="292" spans="1:4" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A292" s="39">
+      <c r="A292" s="33">
         <v>1</v>
       </c>
-      <c r="B292" s="36" t="s">
+      <c r="B292" s="34" t="s">
         <v>542</v>
       </c>
-      <c r="C292" s="36"/>
-      <c r="D292" s="36"/>
+      <c r="C292" s="34"/>
+      <c r="D292" s="34"/>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A293" s="39">
+      <c r="A293" s="33">
         <v>2</v>
       </c>
-      <c r="B293" s="36" t="s">
+      <c r="B293" s="34" t="s">
         <v>543</v>
       </c>
-      <c r="C293" s="36"/>
-      <c r="D293" s="36"/>
+      <c r="C293" s="34"/>
+      <c r="D293" s="34"/>
     </row>
     <row r="294" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A294" s="39">
+      <c r="A294" s="33">
         <v>3</v>
       </c>
-      <c r="B294" s="36" t="s">
+      <c r="B294" s="34" t="s">
         <v>544</v>
       </c>
-      <c r="C294" s="36"/>
-      <c r="D294" s="36"/>
+      <c r="C294" s="34"/>
+      <c r="D294" s="34"/>
     </row>
     <row r="295" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A295" s="39">
+      <c r="A295" s="33">
         <v>4</v>
       </c>
-      <c r="B295" s="36" t="s">
+      <c r="B295" s="34" t="s">
         <v>545</v>
       </c>
-      <c r="C295" s="36"/>
-      <c r="D295" s="36"/>
+      <c r="C295" s="34"/>
+      <c r="D295" s="34"/>
     </row>
     <row r="296" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A296" s="39">
+      <c r="A296" s="33">
         <v>5</v>
       </c>
-      <c r="B296" s="36" t="s">
+      <c r="B296" s="34" t="s">
         <v>546</v>
       </c>
-      <c r="C296" s="36"/>
-      <c r="D296" s="36"/>
+      <c r="C296" s="34"/>
+      <c r="D296" s="34"/>
     </row>
     <row r="297" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A297" s="39">
+      <c r="A297" s="33">
         <v>6</v>
       </c>
-      <c r="B297" s="36" t="s">
+      <c r="B297" s="34" t="s">
         <v>547</v>
       </c>
-      <c r="C297" s="36"/>
-      <c r="D297" s="36"/>
+      <c r="C297" s="34"/>
+      <c r="D297" s="34"/>
     </row>
     <row r="298" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A298" s="39">
+      <c r="A298" s="33">
         <v>7</v>
       </c>
-      <c r="B298" s="36" t="s">
+      <c r="B298" s="34" t="s">
         <v>548</v>
       </c>
-      <c r="C298" s="36"/>
-      <c r="D298" s="36"/>
+      <c r="C298" s="34"/>
+      <c r="D298" s="34"/>
     </row>
     <row r="299" spans="1:4" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A299" s="39">
+      <c r="A299" s="33">
         <v>8</v>
       </c>
-      <c r="B299" s="36" t="s">
+      <c r="B299" s="34" t="s">
         <v>549</v>
       </c>
-      <c r="C299" s="36"/>
-      <c r="D299" s="36"/>
+      <c r="C299" s="34"/>
+      <c r="D299" s="34"/>
     </row>
     <row r="300" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A300" s="39">
+      <c r="A300" s="33">
         <v>9</v>
       </c>
-      <c r="B300" s="36" t="s">
+      <c r="B300" s="34" t="s">
         <v>550</v>
       </c>
-      <c r="C300" s="36"/>
-      <c r="D300" s="36"/>
+      <c r="C300" s="34"/>
+      <c r="D300" s="34"/>
     </row>
     <row r="301" spans="1:4" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A301" s="39">
+      <c r="A301" s="33">
         <v>10</v>
       </c>
-      <c r="B301" s="36" t="s">
+      <c r="B301" s="34" t="s">
         <v>551</v>
       </c>
-      <c r="C301" s="36"/>
-      <c r="D301" s="36"/>
+      <c r="C301" s="34"/>
+      <c r="D301" s="34"/>
     </row>
     <row r="302" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A302" s="39">
+      <c r="A302" s="33">
         <v>11</v>
       </c>
-      <c r="B302" s="36" t="s">
+      <c r="B302" s="34" t="s">
         <v>552</v>
       </c>
-      <c r="C302" s="36"/>
-      <c r="D302" s="36"/>
+      <c r="C302" s="34"/>
+      <c r="D302" s="34"/>
     </row>
     <row r="303" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A303" s="39">
+      <c r="A303" s="33">
         <v>12</v>
       </c>
-      <c r="B303" s="36" t="s">
+      <c r="B303" s="34" t="s">
         <v>553</v>
       </c>
-      <c r="C303" s="36"/>
-      <c r="D303" s="36"/>
+      <c r="C303" s="34"/>
+      <c r="D303" s="34"/>
     </row>
     <row r="304" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A304" s="39">
+      <c r="A304" s="33">
         <v>13</v>
       </c>
-      <c r="B304" s="36" t="s">
+      <c r="B304" s="34" t="s">
         <v>554</v>
       </c>
-      <c r="C304" s="36"/>
-      <c r="D304" s="36"/>
+      <c r="C304" s="34"/>
+      <c r="D304" s="34"/>
     </row>
     <row r="305" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A305" s="39">
+      <c r="A305" s="33">
         <v>14</v>
       </c>
-      <c r="B305" s="36" t="s">
+      <c r="B305" s="34" t="s">
         <v>555</v>
       </c>
-      <c r="C305" s="36"/>
-      <c r="D305" s="36"/>
+      <c r="C305" s="34"/>
+      <c r="D305" s="34"/>
     </row>
     <row r="306" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A306" s="39">
+      <c r="A306" s="33">
         <v>15</v>
       </c>
-      <c r="B306" s="36" t="s">
+      <c r="B306" s="34" t="s">
         <v>556</v>
       </c>
-      <c r="C306" s="36"/>
-      <c r="D306" s="36"/>
+      <c r="C306" s="34"/>
+      <c r="D306" s="34"/>
     </row>
     <row r="307" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A307" s="39">
+      <c r="A307" s="33">
         <v>16</v>
       </c>
-      <c r="B307" s="36" t="s">
+      <c r="B307" s="34" t="s">
         <v>557</v>
       </c>
-      <c r="C307" s="36"/>
-      <c r="D307" s="36"/>
+      <c r="C307" s="34"/>
+      <c r="D307" s="34"/>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A308" s="39">
+      <c r="A308" s="33">
         <v>17</v>
       </c>
-      <c r="B308" s="36" t="s">
+      <c r="B308" s="34" t="s">
         <v>558</v>
       </c>
-      <c r="C308" s="36"/>
-      <c r="D308" s="36"/>
+      <c r="C308" s="34"/>
+      <c r="D308" s="34"/>
     </row>
     <row r="309" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A309" s="39">
+      <c r="A309" s="33">
         <v>18</v>
       </c>
-      <c r="B309" s="36" t="s">
+      <c r="B309" s="34" t="s">
         <v>559</v>
       </c>
-      <c r="C309" s="36"/>
-      <c r="D309" s="36"/>
+      <c r="C309" s="34"/>
+      <c r="D309" s="34"/>
     </row>
     <row r="310" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A310" s="39">
+      <c r="A310" s="33">
         <v>19</v>
       </c>
-      <c r="B310" s="36" t="s">
+      <c r="B310" s="34" t="s">
         <v>560</v>
       </c>
-      <c r="C310" s="36"/>
-      <c r="D310" s="36"/>
+      <c r="C310" s="34"/>
+      <c r="D310" s="34"/>
     </row>
     <row r="311" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A311" s="39">
+      <c r="A311" s="33">
         <v>20</v>
       </c>
-      <c r="B311" s="36" t="s">
+      <c r="B311" s="34" t="s">
         <v>561</v>
       </c>
-      <c r="C311" s="36"/>
-      <c r="D311" s="36"/>
+      <c r="C311" s="34"/>
+      <c r="D311" s="34"/>
     </row>
     <row r="312" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A312" s="39">
+      <c r="A312" s="33">
         <v>21</v>
       </c>
-      <c r="B312" s="36" t="s">
+      <c r="B312" s="34" t="s">
         <v>562</v>
       </c>
-      <c r="C312" s="36"/>
-      <c r="D312" s="36"/>
+      <c r="C312" s="34"/>
+      <c r="D312" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="A269:B269"/>
+    <mergeCell ref="A205:B205"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A214:B214"/>
+    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="A231:B231"/>
+    <mergeCell ref="A248:B248"/>
+    <mergeCell ref="A228:B228"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A157:B157"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="B309:D309"/>
+    <mergeCell ref="B298:D298"/>
+    <mergeCell ref="B299:D299"/>
+    <mergeCell ref="B300:D300"/>
+    <mergeCell ref="B301:D301"/>
+    <mergeCell ref="B302:D302"/>
+    <mergeCell ref="B292:D292"/>
+    <mergeCell ref="B293:D293"/>
+    <mergeCell ref="B294:D294"/>
+    <mergeCell ref="B295:D295"/>
+    <mergeCell ref="B296:D296"/>
+    <mergeCell ref="A187:B187"/>
     <mergeCell ref="B310:D310"/>
     <mergeCell ref="B311:D311"/>
     <mergeCell ref="B312:D312"/>
@@ -14201,46 +14244,6 @@
     <mergeCell ref="B307:D307"/>
     <mergeCell ref="B308:D308"/>
     <mergeCell ref="B297:D297"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="B309:D309"/>
-    <mergeCell ref="B298:D298"/>
-    <mergeCell ref="B299:D299"/>
-    <mergeCell ref="B300:D300"/>
-    <mergeCell ref="B301:D301"/>
-    <mergeCell ref="B302:D302"/>
-    <mergeCell ref="B292:D292"/>
-    <mergeCell ref="B293:D293"/>
-    <mergeCell ref="B294:D294"/>
-    <mergeCell ref="B295:D295"/>
-    <mergeCell ref="B296:D296"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A187:B187"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A157:B157"/>
-    <mergeCell ref="A163:B163"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A180:B180"/>
-    <mergeCell ref="A269:B269"/>
-    <mergeCell ref="A205:B205"/>
-    <mergeCell ref="A209:B209"/>
-    <mergeCell ref="A214:B214"/>
-    <mergeCell ref="A217:B217"/>
-    <mergeCell ref="A231:B231"/>
-    <mergeCell ref="A248:B248"/>
-    <mergeCell ref="A228:B228"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>